<commit_message>
init commit of hub mechanical parts
</commit_message>
<xml_diff>
--- a/hardware/electrical/Hub/Project Outputs for Hub/Hub 1.0 BOM.xlsx
+++ b/hardware/electrical/Hub/Project Outputs for Hub/Hub 1.0 BOM.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brutu\Desktop\LocalGit\seniorproject\hardware\electrical\Hub\Project Outputs for Hub\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>Designator</t>
   </si>
@@ -90,12 +95,6 @@
     <t>.1uF</t>
   </si>
   <si>
-    <t>D1, D3, D4, D5</t>
-  </si>
-  <si>
-    <t>D_LED_LED5MM</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -114,15 +113,6 @@
     <t>1A</t>
   </si>
   <si>
-    <t>H1, H2, H3</t>
-  </si>
-  <si>
-    <t>H_MOUNTHOLE_MOUNTHOLE4MM</t>
-  </si>
-  <si>
-    <t>4mm</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -214,15 +204,6 @@
   </si>
   <si>
     <t>68</t>
-  </si>
-  <si>
-    <t>T1, T2, T3, T4, T5, T6, T7, T8, T9, T10, T11, T12, T13, T14, T15, T16, T17, T18, T19, T20, T21, T22, T23, T24, T25, T26, T27, T28, T29, T30, T31, T32, T33, T34, T35</t>
-  </si>
-  <si>
-    <t>T_TESTPOINT_TESTPOINT1MM</t>
-  </si>
-  <si>
-    <t>1mm</t>
   </si>
   <si>
     <t>U1</t>
@@ -651,9 +632,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -685,396 +668,330 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C4" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3">
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="C10" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C11" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C12" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C13" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C15" s="3">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:G16">
+    <sortCondition ref="E1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>